<commit_message>
Added basic implementation of tool changeover, sequence feeders to minimise number of changeovers required
</commit_message>
<xml_diff>
--- a/input/test_2/setup.xlsx
+++ b/input/test_2/setup.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sam.secher\source\repos\pnp-opt\input\test_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EED01DA-F807-4490-9D27-5F2B37B9056E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BBB927-3C44-4E69-A5D0-8C1405041FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7215" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{44D22B83-19E5-49DB-9A86-332D4007F8A2}"/>
+    <workbookView xWindow="28680" yWindow="-7215" windowWidth="29040" windowHeight="15720" xr2:uid="{44D22B83-19E5-49DB-9A86-332D4007F8A2}"/>
   </bookViews>
   <sheets>
     <sheet name="machine" sheetId="1" r:id="rId1"/>
     <sheet name="feeders" sheetId="2" r:id="rId2"/>
     <sheet name="jobs" sheetId="3" r:id="rId3"/>
     <sheet name="placements" sheetId="4" r:id="rId4"/>
+    <sheet name="tools" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
   <si>
     <t>head_count</t>
   </si>
@@ -255,13 +256,25 @@
   </si>
   <si>
     <t>ComputeBoard</t>
+  </si>
+  <si>
+    <t>nozzle_type</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>nozzle_changeover_s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +284,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -293,14 +313,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{33E745E7-83B8-415E-B182-A41CD2DF8DD9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -632,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAFECAB-9894-4316-8F2A-02B6AAA65DCF}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -699,11 +722,19 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>20</v>
       </c>
     </row>
@@ -787,7 +818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A30C22-82DF-4B90-A229-3B547DB5A8F0}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1625,4 +1656,54 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4F5A5D-BB21-4691-940B-98D8EC29774C}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>